<commit_message>
#2 Added new column <executionStatus> in testData sheet with some changes in KeywordEngine.java
</commit_message>
<xml_diff>
--- a/src/main/java/com/qa/freeCRM/testData/FreeCRM_KeywordDriven.xlsx
+++ b/src/main/java/com/qa/freeCRM/testData/FreeCRM_KeywordDriven.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16245" windowHeight="5970" tabRatio="355" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15840" windowHeight="5970" tabRatio="355" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ConsolidatedSuites" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="107">
   <si>
     <t>TestCase_ID</t>
   </si>
@@ -337,6 +337,12 @@
   </si>
   <si>
     <t>C:\Users\HK-SONY\Selenium_Eclipse_Workspace\FreeCRM_KeywordDriven\src\main\java\com\qa\freeCRM\testData\POM.PNG</t>
+  </si>
+  <si>
+    <t>ExecuteStatus</t>
+  </si>
+  <si>
+    <t>close</t>
   </si>
 </sst>
 </file>
@@ -346,7 +352,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -394,6 +400,14 @@
       <name val="Segoe UI Semibold"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -440,7 +454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -473,6 +487,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -834,10 +851,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -845,12 +862,13 @@
     <col min="1" max="1" width="14" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="65.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="25.5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.5">
       <c r="A1" s="13" t="s">
         <v>11</v>
       </c>
@@ -860,8 +878,9 @@
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H1" s="13"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -880,11 +899,14 @@
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>19</v>
       </c>
@@ -903,8 +925,11 @@
       <c r="F3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>20</v>
       </c>
@@ -923,8 +948,11 @@
       <c r="F4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>21</v>
       </c>
@@ -943,8 +971,11 @@
       <c r="F5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -961,8 +992,11 @@
         <v>79</v>
       </c>
       <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>23</v>
       </c>
@@ -981,8 +1015,11 @@
       <c r="F7" s="8" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G7" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>23</v>
       </c>
@@ -1001,8 +1038,11 @@
       <c r="F8" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G8" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>24</v>
       </c>
@@ -1021,8 +1061,11 @@
       <c r="F9" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G9" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>25</v>
       </c>
@@ -1041,8 +1084,11 @@
       <c r="F10" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>44</v>
       </c>
@@ -1061,8 +1107,11 @@
       <c r="F11" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G11" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>45</v>
       </c>
@@ -1081,8 +1130,11 @@
       <c r="F12" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>46</v>
       </c>
@@ -1101,8 +1153,11 @@
       <c r="F13" s="5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="G13" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" customFormat="1" ht="135" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>47</v>
       </c>
@@ -1121,8 +1176,11 @@
       <c r="F14" s="6" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G14" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>48</v>
       </c>
@@ -1141,8 +1199,11 @@
       <c r="F15" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G15" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>95</v>
       </c>
@@ -1161,8 +1222,11 @@
       <c r="F16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G16" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>49</v>
       </c>
@@ -1181,8 +1245,11 @@
       <c r="F17" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G17" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>50</v>
       </c>
@@ -1201,8 +1268,11 @@
       <c r="F18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
@@ -1221,8 +1291,11 @@
       <c r="F19" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G19" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>51</v>
       </c>
@@ -1241,8 +1314,11 @@
       <c r="F20" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G20" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
@@ -1261,8 +1337,11 @@
       <c r="F21" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>53</v>
       </c>
@@ -1281,8 +1360,11 @@
       <c r="F22" s="10">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G22" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>54</v>
       </c>
@@ -1301,8 +1383,11 @@
       <c r="F23" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G23" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>55</v>
       </c>
@@ -1321,8 +1406,11 @@
       <c r="F24" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G24" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>55</v>
       </c>
@@ -1341,8 +1429,11 @@
       <c r="F25" s="4">
         <v>1992</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>56</v>
       </c>
@@ -1361,8 +1452,11 @@
       <c r="F26" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G26" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>66</v>
       </c>
@@ -1381,15 +1475,20 @@
       <c r="F27" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G27" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B28" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C28" s="7"/>
+      <c r="C28" s="7" t="s">
+        <v>106</v>
+      </c>
       <c r="D28" s="2" t="s">
         <v>59</v>
       </c>
@@ -1398,11 +1497,14 @@
       </c>
       <c r="F28" t="s">
         <v>59</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F13" r:id="rId1"/>

</xml_diff>